<commit_message>
use data public budget
</commit_message>
<xml_diff>
--- a/data-raw/df-vars-matched.xlsx
+++ b/data-raw/df-vars-matched.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">input</t>
   </si>
@@ -26,70 +26,28 @@
     <t xml:space="preserve">variables</t>
   </si>
   <si>
-    <t xml:space="preserve">农业机械总动力</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_zdl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">大中型拖拉机</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_dztlj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">大中型拖拉机配套农具</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_dztlj_pt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">小型拖拉机</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_xtlj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">农用水泵</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_nysb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">联合收获机</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_lhshj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">机动脱粒机</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_jdtlj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">节水灌溉类机械</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_jsgg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">机耕面积</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_jgmj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">机播面积</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_jbmj</t>
-  </si>
-  <si>
-    <t xml:space="preserve">机收面积</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v7_sctj_nyjx_jsmj</t>
+    <t xml:space="preserve">合计</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v6_cz_yszc_hj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">教育</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v6_cz_yszc_jy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">科学技术</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v6_cz_yszc_kxjs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">农林水</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v6_cz_yszc_nls</t>
   </si>
 </sst>
 </file>
@@ -491,104 +449,6 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="b">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="b">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" t="b">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="b">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="b">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="b">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" t="b">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
use data hi-tech industry
</commit_message>
<xml_diff>
--- a/data-raw/df-vars-matched.xlsx
+++ b/data-raw/df-vars-matched.xlsx
@@ -26,22 +26,22 @@
     <t xml:space="preserve">variables</t>
   </si>
   <si>
-    <t xml:space="preserve">企业数</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4_cy_scjy_qys</t>
-  </si>
-  <si>
-    <t xml:space="preserve">主营业务收入</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4_cy_scjy_zyyw</t>
-  </si>
-  <si>
-    <t xml:space="preserve">利润总额</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4_cy_scjy_lrze</t>
+    <t xml:space="preserve">出口贸易额</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v4_cy_my_ck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">进口贸易额</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v4_cy_my_jk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">贸易总额</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v4_cy_my_jck</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
livestock tab1 tidy  finished
</commit_message>
<xml_diff>
--- a/data-raw/df-vars-matched.xlsx
+++ b/data-raw/df-vars-matched.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t xml:space="preserve">input</t>
   </si>
@@ -26,22 +26,85 @@
     <t xml:space="preserve">variables</t>
   </si>
   <si>
-    <t xml:space="preserve">出口贸易额</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4_cy_my_ck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">进口贸易额</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4_cy_my_jk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">贸易总额</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4_cy_my_jck</t>
+    <t xml:space="preserve">总数</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种牛场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_znc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种奶牛场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_znnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种肉牛场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zrnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种水牛场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zsnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种牦牛场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zhnc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种马场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zmc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种猪场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zzc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种羊场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zyc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种绵羊场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zmyc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种细毛羊场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zxmyc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种山羊场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zsyc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种绒山羊场</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v8_t1_zcqc_zmsyc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">种乳牛场</t>
   </si>
 </sst>
 </file>
@@ -429,6 +492,160 @@
         <v>9</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="b">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="b">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="b">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="b">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="b">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="b">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="b">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" t="b">
+        <v>1</v>
+      </c>
+      <c r="D14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="b">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>